<commit_message>
new data + added per 32 stats
</commit_message>
<xml_diff>
--- a/results/shot_chart_2022.xlsx
+++ b/results/shot_chart_2022.xlsx
@@ -486,22 +486,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="E2" t="n">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="F2" t="n">
-        <v>53.9</v>
+        <v>52.5</v>
       </c>
       <c r="G2" t="n">
-        <v>48</v>
+        <v>45.7</v>
       </c>
     </row>
     <row r="3">
@@ -515,16 +515,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>37.5</v>
+        <v>30</v>
       </c>
       <c r="G3" t="n">
-        <v>28.6</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="4">
@@ -535,19 +535,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="5">
@@ -581,19 +581,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" t="n">
-        <v>26.7</v>
+        <v>26.3</v>
       </c>
       <c r="G6" t="n">
-        <v>26.7</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="7">
@@ -604,19 +604,19 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>7.1</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="8">
@@ -630,16 +630,16 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E8" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F8" t="n">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
       <c r="G8" t="n">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="9">
@@ -653,16 +653,16 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" t="n">
-        <v>15.4</v>
+        <v>13.3</v>
       </c>
       <c r="G9" t="n">
-        <v>15.4</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="10">
@@ -699,16 +699,16 @@
         <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
-        <v>27.3</v>
+        <v>23.1</v>
       </c>
       <c r="G11" t="n">
-        <v>27.3</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="12">
@@ -745,16 +745,16 @@
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F13" t="n">
-        <v>13.3</v>
+        <v>11.8</v>
       </c>
       <c r="G13" t="n">
-        <v>13.3</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="14">
@@ -765,19 +765,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>16.7</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,7 +861,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -870,44 +870,44 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -930,24 +930,47 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -962,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1018,16 +1041,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G2" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -1055,13 +1078,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1070,55 +1093,78 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1183,22 +1229,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D2" t="n">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="E2" t="n">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="F2" t="n">
-        <v>53.8</v>
+        <v>54.2</v>
       </c>
       <c r="G2" t="n">
-        <v>49</v>
+        <v>49.7</v>
       </c>
     </row>
     <row r="3">
@@ -1209,19 +1255,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>33.3</v>
+        <v>37.5</v>
       </c>
       <c r="G3" t="n">
-        <v>33.3</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="4">
@@ -1232,19 +1278,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>28.6</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="5">
@@ -1255,19 +1301,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="n">
-        <v>23.5</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>23.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -1278,19 +1324,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="n">
-        <v>23.5</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
-        <v>23.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -1304,16 +1350,16 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F7" t="n">
-        <v>18.2</v>
+        <v>14.3</v>
       </c>
       <c r="G7" t="n">
-        <v>18.2</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="8">
@@ -1324,19 +1370,19 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" t="n">
-        <v>28</v>
+        <v>29.6</v>
       </c>
       <c r="G8" t="n">
-        <v>28</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="9">
@@ -1350,16 +1396,16 @@
         <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" t="n">
-        <v>17.6</v>
+        <v>16.7</v>
       </c>
       <c r="G9" t="n">
-        <v>17.6</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="10">
@@ -1373,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20</v>
+        <v>14.3</v>
       </c>
       <c r="G10" t="n">
-        <v>20</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="11">
@@ -1396,10 +1442,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1419,16 +1465,16 @@
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>66.7</v>
+        <v>50</v>
       </c>
       <c r="G12" t="n">
-        <v>66.7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -1439,19 +1485,19 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" t="n">
+        <v>44.4</v>
+      </c>
+      <c r="G13" t="n">
         <v>41.2</v>
-      </c>
-      <c r="G13" t="n">
-        <v>37.5</v>
       </c>
     </row>
     <row r="14">
@@ -1465,16 +1511,16 @@
         <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
-        <v>57.1</v>
+        <v>44.4</v>
       </c>
       <c r="G14" t="n">
-        <v>57.1</v>
+        <v>44.4</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1541,19 +1587,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>52.6</v>
+        <v>56</v>
       </c>
       <c r="G2" t="n">
-        <v>47.1</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="3">
@@ -1581,53 +1627,53 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1636,44 +1682,44 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>66.7</v>
+        <v>50</v>
       </c>
       <c r="G6" t="n">
-        <v>66.7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1682,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1696,10 +1742,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1708,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1719,25 +1765,48 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>13</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>100</v>
-      </c>
-      <c r="G10" t="n">
-        <v>100</v>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1804,19 +1873,19 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F2" t="n">
-        <v>50</v>
+        <v>47.7</v>
       </c>
       <c r="G2" t="n">
-        <v>47.4</v>
+        <v>45.2</v>
       </c>
     </row>
     <row r="3">
@@ -1899,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1919,19 +1988,19 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G7" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -2021,19 +2090,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E2" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F2" t="n">
-        <v>78.59999999999999</v>
+        <v>79.2</v>
       </c>
       <c r="G2" t="n">
-        <v>75</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="3">
@@ -2093,16 +2162,16 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>33.3</v>
+        <v>28.6</v>
       </c>
       <c r="G5" t="n">
-        <v>33.3</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="6">
@@ -2139,16 +2208,16 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>11.1</v>
+        <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>11.1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -2159,19 +2228,19 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
-        <v>36.4</v>
+        <v>41.7</v>
       </c>
       <c r="G8" t="n">
-        <v>36.4</v>
+        <v>41.7</v>
       </c>
     </row>
     <row r="9">
@@ -2208,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2373,22 +2442,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E2" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F2" t="n">
-        <v>43.8</v>
+        <v>46.5</v>
       </c>
       <c r="G2" t="n">
-        <v>33.3</v>
+        <v>37.8</v>
       </c>
     </row>
     <row r="3">
@@ -2540,7 +2609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2587,7 +2656,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -2610,24 +2679,70 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>10</v>
       </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2642,7 +2757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2698,27 +2813,27 @@
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>66.7</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -2727,15 +2842,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -2758,47 +2873,70 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>33.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>13</v>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
         <v>50</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G7" t="n">
         <v>50</v>
       </c>
     </row>
@@ -2813,7 +2951,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2866,19 +3004,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
-        <v>37.5</v>
+        <v>40.7</v>
       </c>
       <c r="G2" t="n">
-        <v>34.8</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="3">
@@ -3021,24 +3159,47 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>12</v>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
         <v>3</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>3</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3053,7 +3214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3103,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -3112,10 +3273,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>33.3</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -3192,7 +3353,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -3215,13 +3376,13 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -3230,32 +3391,78 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>13</v>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>